<commit_message>
Changed headers in all tests in test_files folder
</commit_message>
<xml_diff>
--- a/test_files/data_samples/21-genes_50-edges_Dahlquist-data_MM_estimation.xlsx
+++ b/test_files/data_samples/21-genes_50-edges_Dahlquist-data_MM_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="27600" windowHeight="8655" tabRatio="644" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="27600" windowHeight="8655" tabRatio="644"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">network!$A$1:$V$22</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -158,9 +158,6 @@
     <t>degradation_rate</t>
   </si>
   <si>
-    <t>regulators/controllers</t>
-  </si>
-  <si>
     <t>estimate_params</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>threshold_b</t>
+  </si>
+  <si>
+    <t>targets/regulators</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -236,7 +236,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -644,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -952,7 +951,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
@@ -960,7 +959,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -992,7 +991,7 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="9">
         <v>15</v>
@@ -1066,7 +1065,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1120,9 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1131,11 +1128,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>43</v>
+      <c r="A1" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6201,7 +6198,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
@@ -7732,7 +7729,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Preliminary work so that readInputSheet reads ALL files in the test_files directory, not just the sixteen_tests, etc.
</commit_message>
<xml_diff>
--- a/test_files/data_samples/21-genes_50-edges_Dahlquist-data_MM_estimation.xlsx
+++ b/test_files/data_samples/21-genes_50-edges_Dahlquist-data_MM_estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="27600" windowHeight="8655" tabRatio="644"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="27600" windowHeight="8655" tabRatio="644" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="51">
   <si>
     <t>CIN5</t>
   </si>
@@ -146,9 +146,6 @@
     <t>dzap1</t>
   </si>
   <si>
-    <t>Sigmoid</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -174,6 +171,15 @@
   </si>
   <si>
     <t>targets/regulators</t>
+  </si>
+  <si>
+    <t>production_function</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>L_curve</t>
   </si>
 </sst>
 </file>
@@ -643,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -655,10 +661,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -870,10 +876,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -888,18 +894,6 @@
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -949,161 +943,169 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
       <c r="B13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="9">
         <v>15</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>30</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="8">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B16" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
         <v>6</v>
       </c>
-      <c r="E16">
-        <v>8</v>
-      </c>
       <c r="F16">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>25</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <v>35</v>
+      </c>
+      <c r="J18">
+        <v>40</v>
+      </c>
+      <c r="K18">
         <v>45</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
-      <c r="F17">
-        <v>20</v>
-      </c>
-      <c r="G17">
-        <v>25</v>
-      </c>
-      <c r="H17">
-        <v>30</v>
-      </c>
-      <c r="I17">
-        <v>35</v>
-      </c>
-      <c r="J17">
-        <v>40</v>
-      </c>
-      <c r="K17">
-        <v>45</v>
-      </c>
-      <c r="L17">
+      <c r="L18">
         <v>50</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>55</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>60</v>
       </c>
     </row>
@@ -1124,15 +1126,15 @@
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1327,10 +1329,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1519,7 +1521,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7">
         <v>15</v>
@@ -2504,7 +2506,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7">
         <v>15</v>
@@ -3423,7 +3425,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7">
         <v>15</v>
@@ -4342,7 +4344,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7">
         <v>15</v>
@@ -5261,7 +5263,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7">
         <v>15</v>
@@ -6198,7 +6200,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
@@ -7729,7 +7731,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>

</xml_diff>